<commit_message>
add illegal descendant rules to schematron
</commit_message>
<xml_diff>
--- a/reports/null_element_counts.xlsx
+++ b/reports/null_element_counts.xlsx
@@ -200,8 +200,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,22 +256,23 @@
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -612,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -623,13 +633,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>